<commit_message>
creating jpg and tidying up inventory creation
</commit_message>
<xml_diff>
--- a/2022/data/processed/CENCOOS.xlsx
+++ b/2022/data/processed/CENCOOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2022\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A340593-71CF-44C9-9C31-5801AF928647}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD352ED-A381-4D26-860C-1E8A51C268CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,12 @@
     <definedName name="RAFunding">#REF!</definedName>
     <definedName name="sector">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="159">
   <si>
     <t>Station ID</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Chevron Dock Pier Station</t>
   </si>
   <si>
-    <t>yp</t>
-  </si>
-  <si>
     <t>sea_water_temperature(2m), sea_water_salinity(2m), mass_concentration_of_oxygen_in_sea_water(2m), sea_water_ph_measured_on_total_scale(2m), mass_concentration_of_chlorophyll_in_sea_water(2m), sea_water_turbidity(2m), sea_water_pressure(2m)</t>
   </si>
   <si>
@@ -620,6 +617,12 @@
   </si>
   <si>
     <t>MBARI Power Buoy</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -985,9 +988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1015,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1077,7 +1080,7 @@
     </row>
     <row r="2" spans="1:27" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>33</v>
@@ -1104,7 +1107,7 @@
         <v>39813</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>39</v>
@@ -1142,7 +1145,7 @@
     </row>
     <row r="3" spans="1:27" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>46</v>
@@ -1169,13 +1172,13 @@
         <v>2003</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>39</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>41</v>
@@ -1190,7 +1193,7 @@
         <v>43</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
@@ -1205,17 +1208,17 @@
     </row>
     <row r="4" spans="1:27" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="F4" s="10">
         <v>40.43</v>
@@ -1230,7 +1233,7 @@
         <v>38930</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1251,7 +1254,7 @@
         <v>41</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
@@ -1266,17 +1269,17 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="10">
         <v>40.793939999999999</v>
@@ -1291,7 +1294,7 @@
         <v>44805</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
@@ -1321,17 +1324,17 @@
     </row>
     <row r="6" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="F6" s="10">
         <v>38.32</v>
@@ -1340,34 +1343,34 @@
         <v>-123.07</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I6" s="4">
         <v>2007</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -1382,19 +1385,19 @@
     </row>
     <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F7" s="10">
         <v>38.32</v>
@@ -1403,34 +1406,34 @@
         <v>-123.07</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="4">
         <v>2003</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -1445,17 +1448,17 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="10">
         <v>38.3185</v>
@@ -1470,22 +1473,22 @@
         <v>44713</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="12"/>
@@ -1502,17 +1505,17 @@
     </row>
     <row r="9" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F9" s="10">
         <v>36.161999999999999</v>
@@ -1521,34 +1524,34 @@
         <v>-122.8939</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="11">
         <v>41790</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>90</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1563,19 +1566,19 @@
     </row>
     <row r="10" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="F10" s="10">
         <v>38.07</v>
@@ -1590,28 +1593,28 @@
         <v>39499</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -1626,19 +1629,19 @@
     </row>
     <row r="11" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="F11" s="10">
         <v>37.89</v>
@@ -1653,28 +1656,28 @@
         <v>37561</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -1689,19 +1692,19 @@
     </row>
     <row r="12" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F12" s="10">
         <v>37.81</v>
@@ -1716,28 +1719,28 @@
         <v>39872</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="P12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="Q12" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1752,17 +1755,17 @@
     </row>
     <row r="13" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="10">
         <v>37.799999999999997</v>
@@ -1775,28 +1778,28 @@
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="N13" s="4" t="s">
+      <c r="O13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q13" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q13" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -1811,17 +1814,17 @@
     </row>
     <row r="14" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F14" s="10">
         <v>37.799999999999997</v>
@@ -1836,25 +1839,25 @@
         <v>42614</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="K14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q14" s="12"/>
       <c r="R14" s="4"/>
@@ -1870,17 +1873,17 @@
     </row>
     <row r="15" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" s="10">
         <v>36.96</v>
@@ -1895,28 +1898,28 @@
         <v>40858</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q15" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="Q15" s="12" t="s">
-        <v>115</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
@@ -1931,17 +1934,17 @@
     </row>
     <row r="16" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F16" s="10">
         <v>36.96</v>
@@ -1956,25 +1959,25 @@
         <v>42217</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q16" s="12"/>
       <c r="R16" s="4"/>
@@ -1990,19 +1993,19 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="F17" s="10">
         <v>36.799999999999997</v>
@@ -2017,28 +2020,28 @@
         <v>40424</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O17" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="Q17" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="Q17" s="12" t="s">
-        <v>125</v>
       </c>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -2053,19 +2056,19 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="4">
         <v>46092</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F18" s="10">
         <v>36.758000000000003</v>
@@ -2074,34 +2077,34 @@
         <v>-122.029</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I18" s="4">
         <v>1991</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q18" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -2116,45 +2119,45 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F19" s="10">
         <v>36.744</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I19" s="15">
         <v>44425</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="12"/>
@@ -2171,17 +2174,17 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="F20" s="10">
         <v>36.618600000000001</v>
@@ -2190,32 +2193,32 @@
         <v>-121.9015</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K20" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="P20" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="P20" s="4" t="s">
+      <c r="Q20" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
@@ -2230,19 +2233,19 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="F21" s="10">
         <v>35.369999999999997</v>
@@ -2257,28 +2260,28 @@
         <v>39083</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O21" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q21" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q21" s="17" t="s">
-        <v>145</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -2293,17 +2296,17 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F22" s="10">
         <v>35.333820000000003</v>
@@ -2318,26 +2321,26 @@
         <v>43363</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
@@ -2352,19 +2355,19 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="F23" s="10">
         <v>35.17</v>
@@ -2379,28 +2382,28 @@
         <v>38473</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q23" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
@@ -2570,17 +2573,17 @@
     </row>
     <row r="3" spans="1:27" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="10">
         <v>40.81</v>
@@ -2598,25 +2601,25 @@
         <v>38</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="O3" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>43</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -2629,19 +2632,19 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="255" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="F4" s="10">
         <v>39.6</v>
@@ -2650,34 +2653,34 @@
         <v>-123.79</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="4">
         <v>2007</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
@@ -2690,19 +2693,19 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="F5" s="10">
         <v>38.19</v>
@@ -2711,7 +2714,7 @@
         <v>-122.93</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" s="11">
         <v>41428</v>
@@ -2720,25 +2723,25 @@
         <v>38</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="Q5" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
@@ -2753,19 +2756,19 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="F6" s="10">
         <v>36.61</v>
@@ -2780,28 +2783,28 @@
         <v>42128</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="O6" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="Q6" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>

</xml_diff>